<commit_message>
recursive growth strategy is introduced
* `Recursive` growth strategy is defined and implemented.
* Benchmarks extended by including the `Recursive` strategy and adding the `append` benchmark.
* `IntoFragments` trait is defined to allow overloading in `append` function.
* Documentation is updated accordingly.
</commit_message>
<xml_diff>
--- a/benches/results/grow.xlsx
+++ b/benches/results/grow.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\uurdev\orx\orx-split-vec\benches\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB84CEB-D57A-41C2-BB9F-8D1B1444CA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAD61C2-6158-411D-B806-28DFA4EA2332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="1" xr2:uid="{201707E4-C870-4993-88CE-4A7BD9846E2B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="2" xr2:uid="{201707E4-C870-4993-88CE-4A7BD9846E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="grow" sheetId="1" r:id="rId1"/>
     <sheet name="serial-access" sheetId="6" r:id="rId2"/>
     <sheet name="random-access" sheetId="5" r:id="rId3"/>
+    <sheet name="append-expand" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="12">
   <si>
     <t>std_vec_with_capacity</t>
   </si>
@@ -65,6 +66,15 @@
   </si>
   <si>
     <t>number of elements</t>
+  </si>
+  <si>
+    <t>split_vec_recursive</t>
+  </si>
+  <si>
+    <t>std_vec_with_exact_capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -110,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -374,11 +384,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1" tint="0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1" tint="0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1" tint="0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -401,12 +569,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -484,6 +646,54 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -509,9 +719,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -549,7 +759,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -655,7 +865,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -797,7 +1007,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1066,44 +1276,44 @@
         <f>C1</f>
         <v>number of elements</v>
       </c>
-      <c r="D26" s="8" t="str">
+      <c r="D26" s="35" t="str">
         <f>D1</f>
         <v>u64 x 1</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8" t="str">
+      <c r="E26" s="35"/>
+      <c r="F26" s="35" t="str">
         <f>F1</f>
         <v>u64 x 16</v>
       </c>
-      <c r="G26" s="9"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="24">
         <f>C2</f>
         <v>1024</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="25">
         <f>D2</f>
         <v>2.0407000000000003E-3</v>
       </c>
-      <c r="E27" s="35">
+      <c r="E27" s="33">
         <f>D27/D$27</f>
         <v>1</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="25">
         <f>F2</f>
         <v>1.0648999999999999E-2</v>
       </c>
-      <c r="G27" s="32">
+      <c r="G27" s="30">
         <f>F27/F$27</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="3">
@@ -1122,13 +1332,13 @@
         <f t="shared" ref="F28" si="2">F3</f>
         <v>2.0448000000000001E-2</v>
       </c>
-      <c r="G28" s="33">
+      <c r="G28" s="31">
         <f t="shared" si="1"/>
         <v>1.9201802986195891</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="3">
@@ -1147,63 +1357,63 @@
         <f t="shared" ref="F29" si="3">F4</f>
         <v>1.2414E-2</v>
       </c>
-      <c r="G29" s="33">
+      <c r="G29" s="31">
         <f t="shared" si="1"/>
         <v>1.1657432622781483</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="30">
+      <c r="C30" s="28">
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="29">
         <f t="shared" si="0"/>
         <v>3.2768000000000003E-3</v>
       </c>
-      <c r="E30" s="36">
+      <c r="E30" s="34">
         <f t="shared" si="1"/>
         <v>1.6057235262409957</v>
       </c>
-      <c r="F30" s="31">
+      <c r="F30" s="29">
         <f t="shared" ref="F30" si="4">F5</f>
         <v>1.5285E-2</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="32">
         <f t="shared" si="1"/>
         <v>1.4353460418818671</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="24">
         <f t="shared" si="0"/>
         <v>16384</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D31" s="25">
         <f t="shared" si="0"/>
         <v>3.1682000000000002E-2</v>
       </c>
-      <c r="E31" s="35">
+      <c r="E31" s="33">
         <f>D31/D$31</f>
         <v>1</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="25">
         <f t="shared" ref="F31" si="5">F6</f>
         <v>0.54661000000000004</v>
       </c>
-      <c r="G31" s="32">
+      <c r="G31" s="30">
         <f t="shared" ref="G31:G34" si="6">F31/F$31</f>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="3">
@@ -1222,13 +1432,13 @@
         <f t="shared" ref="F32" si="8">F7</f>
         <v>0.80680999999999992</v>
       </c>
-      <c r="G32" s="33">
+      <c r="G32" s="31">
         <f t="shared" si="6"/>
         <v>1.4760249538061869</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="3">
@@ -1247,63 +1457,63 @@
         <f t="shared" ref="F33" si="9">F8</f>
         <v>0.26712999999999998</v>
       </c>
-      <c r="G33" s="33">
+      <c r="G33" s="31">
         <f t="shared" si="6"/>
         <v>0.48870309727227818</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C34" s="28">
         <f t="shared" si="0"/>
         <v>16384</v>
       </c>
-      <c r="D34" s="31">
+      <c r="D34" s="29">
         <f t="shared" si="0"/>
         <v>3.9875000000000001E-2</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <f t="shared" si="7"/>
         <v>1.258601098415504</v>
       </c>
-      <c r="F34" s="31">
+      <c r="F34" s="29">
         <f t="shared" ref="F34" si="10">F9</f>
         <v>0.40232000000000001</v>
       </c>
-      <c r="G34" s="34">
+      <c r="G34" s="32">
         <f t="shared" si="6"/>
         <v>0.73602751504729147</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="24">
         <f t="shared" si="0"/>
         <v>262144</v>
       </c>
-      <c r="D35" s="27">
+      <c r="D35" s="25">
         <f t="shared" si="0"/>
         <v>0.84829999999999994</v>
       </c>
-      <c r="E35" s="35">
+      <c r="E35" s="33">
         <f>D35/D$35</f>
         <v>1</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="25">
         <f t="shared" ref="F35" si="11">F10</f>
         <v>9.4764999999999997</v>
       </c>
-      <c r="G35" s="32">
+      <c r="G35" s="30">
         <f t="shared" ref="G35:G38" si="12">F35/F$35</f>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="3">
@@ -1322,13 +1532,13 @@
         <f t="shared" ref="F36" si="14">F11</f>
         <v>16.956</v>
       </c>
-      <c r="G36" s="33">
+      <c r="G36" s="31">
         <f t="shared" si="12"/>
         <v>1.7892681897324962</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C37" s="3">
@@ -1347,63 +1557,63 @@
         <f t="shared" ref="F37" si="15">F12</f>
         <v>6.6300999999999997</v>
       </c>
-      <c r="G37" s="33">
+      <c r="G37" s="31">
         <f t="shared" si="12"/>
         <v>0.69963594153959796</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="30">
+      <c r="C38" s="28">
         <f t="shared" si="0"/>
         <v>262144</v>
       </c>
-      <c r="D38" s="31">
+      <c r="D38" s="29">
         <f t="shared" si="0"/>
         <v>0.81852000000000003</v>
       </c>
-      <c r="E38" s="36">
+      <c r="E38" s="34">
         <f t="shared" si="13"/>
         <v>0.96489449487209722</v>
       </c>
-      <c r="F38" s="31">
+      <c r="F38" s="29">
         <f t="shared" ref="F38:F42" si="16">F13</f>
         <v>9.8628999999999998</v>
       </c>
-      <c r="G38" s="34">
+      <c r="G38" s="32">
         <f t="shared" si="12"/>
         <v>1.0407745475650292</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="24">
         <f t="shared" ref="C39" si="17">C14</f>
         <v>4194304</v>
       </c>
-      <c r="D39" s="27">
+      <c r="D39" s="25">
         <f t="shared" ref="D39" si="18">D14</f>
         <v>14.356</v>
       </c>
-      <c r="E39" s="35">
+      <c r="E39" s="33">
         <f>D39/D$39</f>
         <v>1</v>
       </c>
-      <c r="F39" s="27">
+      <c r="F39" s="25">
         <f t="shared" si="16"/>
         <v>162.96</v>
       </c>
-      <c r="G39" s="32">
+      <c r="G39" s="30">
         <f t="shared" ref="G39:G42" si="19">F39/F$39</f>
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="3">
@@ -1422,13 +1632,13 @@
         <f t="shared" si="16"/>
         <v>297.17</v>
       </c>
-      <c r="G40" s="33">
+      <c r="G40" s="31">
         <f t="shared" si="19"/>
         <v>1.8235763377515954</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C41" s="3">
@@ -1447,51 +1657,51 @@
         <f t="shared" si="16"/>
         <v>147.15</v>
       </c>
-      <c r="G41" s="33">
+      <c r="G41" s="31">
         <f t="shared" si="19"/>
         <v>0.90298232695139913</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="30">
+      <c r="C42" s="28">
         <f t="shared" ref="C42" si="25">C17</f>
         <v>4194304</v>
       </c>
-      <c r="D42" s="31">
+      <c r="D42" s="29">
         <f t="shared" ref="D42" si="26">D17</f>
         <v>15.792999999999999</v>
       </c>
-      <c r="E42" s="36">
+      <c r="E42" s="34">
         <f t="shared" si="22"/>
         <v>1.1000975202006129</v>
       </c>
-      <c r="F42" s="31">
+      <c r="F42" s="29">
         <f t="shared" si="16"/>
         <v>154.85</v>
       </c>
-      <c r="G42" s="34">
+      <c r="G42" s="32">
         <f t="shared" si="19"/>
         <v>0.95023318605792828</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1537,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7F03E0-41BF-4C59-ABB3-4A77BB8DE656}">
-  <dimension ref="B1:N34"/>
+  <dimension ref="B1:N41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,7 +1784,7 @@
         <v>1.3843E-3</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F7" si="0">J2/1000</f>
+        <f t="shared" ref="F2:F9" si="0">J2/1000</f>
         <v>5.8246000000000001E-3</v>
       </c>
       <c r="H2">
@@ -1592,7 +1802,7 @@
         <v>1024</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D10" si="1">H3/1000</f>
+        <f t="shared" ref="D3:D13" si="1">H3/1000</f>
         <v>1.1573E-3</v>
       </c>
       <c r="F3">
@@ -1630,65 +1840,65 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>16384</v>
+        <v>1024</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>2.2847000000000003E-2</v>
+        <v>1.1973999999999999E-3</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0.10091</v>
+        <v>6.0742000000000001E-3</v>
       </c>
       <c r="H5">
-        <v>22.847000000000001</v>
+        <v>1.1974</v>
       </c>
       <c r="J5">
-        <v>100.91</v>
+        <v>6.0742000000000003</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>16384</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>1.9015000000000001E-2</v>
+        <v>2.2847000000000003E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0.10249999999999999</v>
+        <v>0.10091</v>
       </c>
       <c r="H6">
-        <v>19.015000000000001</v>
+        <v>22.847000000000001</v>
       </c>
       <c r="J6">
-        <v>102.5</v>
+        <v>100.91</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>16384</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>1.9E-2</v>
+        <v>1.9015000000000001E-2</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>0.10249999999999999</v>
       </c>
       <c r="H7">
-        <v>19</v>
+        <v>19.015000000000001</v>
       </c>
       <c r="J7">
         <v>102.5</v>
@@ -1696,470 +1906,650 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>0.36402999999999996</v>
+        <v>1.9E-2</v>
       </c>
       <c r="F8">
-        <v>2.4842</v>
+        <f t="shared" si="0"/>
+        <v>0.10249999999999999</v>
       </c>
       <c r="H8">
-        <v>364.03</v>
+        <v>19</v>
+      </c>
+      <c r="J8">
+        <v>102.5</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>0.31098999999999999</v>
+        <v>1.9010000000000003E-2</v>
       </c>
       <c r="F9">
-        <v>2.5592999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.10340000000000001</v>
       </c>
       <c r="H9">
-        <v>310.99</v>
+        <v>19.010000000000002</v>
+      </c>
+      <c r="J9">
+        <v>103.4</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>262144</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>0.30449999999999999</v>
+        <v>0.36402999999999996</v>
       </c>
       <c r="F10">
-        <v>2.5009000000000001</v>
+        <v>2.4842</v>
       </c>
       <c r="H10">
-        <v>304.5</v>
+        <v>364.03</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>4194304</v>
+        <v>262144</v>
       </c>
       <c r="D11">
-        <v>6.6346999999999996</v>
+        <f t="shared" si="1"/>
+        <v>0.31098999999999999</v>
       </c>
       <c r="F11">
-        <v>39.786999999999999</v>
+        <v>2.5592999999999999</v>
+      </c>
+      <c r="H11">
+        <v>310.99</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>4194304</v>
+        <v>262144</v>
       </c>
       <c r="D12">
-        <v>5.8848000000000003</v>
+        <f t="shared" si="1"/>
+        <v>0.30449999999999999</v>
       </c>
       <c r="F12">
-        <v>40.158000000000001</v>
+        <v>2.5009000000000001</v>
+      </c>
+      <c r="H12">
+        <v>304.5</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>262144</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>0.30580000000000002</v>
+      </c>
+      <c r="F13">
+        <v>2.5104000000000002</v>
+      </c>
+      <c r="H13">
+        <v>305.8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>4194304</v>
+      </c>
+      <c r="D14">
+        <v>6.6346999999999996</v>
+      </c>
+      <c r="F14">
+        <v>39.786999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>4194304</v>
+      </c>
+      <c r="D15">
+        <v>5.8848000000000003</v>
+      </c>
+      <c r="F15">
+        <v>40.158000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="C13">
+      <c r="C16">
         <v>4194304</v>
       </c>
-      <c r="D13">
+      <c r="D16">
         <v>5.6269999999999998</v>
       </c>
-      <c r="F13">
+      <c r="F16">
         <v>40.21</v>
       </c>
     </row>
-    <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>4194304</v>
+      </c>
+      <c r="D17">
+        <v>5.6340000000000003</v>
+      </c>
+      <c r="F17">
+        <v>40.17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="7" t="str">
-        <f t="shared" ref="C22:D34" si="2">C1</f>
+      <c r="C25" s="7" t="str">
+        <f>C1</f>
         <v>number of elements</v>
       </c>
-      <c r="D22" s="8" t="str">
-        <f t="shared" si="2"/>
+      <c r="D25" s="35" t="str">
+        <f>D1</f>
         <v>u64 x 1</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8" t="str">
-        <f t="shared" ref="F22:F34" si="3">F1</f>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35" t="str">
+        <f>F1</f>
         <v>u64 x 16</v>
       </c>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="str">
+      <c r="G25" s="36"/>
+    </row>
+    <row r="26" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="str">
         <f>B2</f>
         <v>std_vec</v>
       </c>
-      <c r="C23" s="11">
-        <f t="shared" si="2"/>
+      <c r="C26" s="9">
+        <f>C2</f>
         <v>1024</v>
       </c>
-      <c r="D23" s="12">
-        <f t="shared" si="2"/>
+      <c r="D26" s="10">
+        <f>D2</f>
         <v>1.3843E-3</v>
       </c>
-      <c r="E23" s="13">
-        <f>D23/D$23</f>
-        <v>1</v>
-      </c>
-      <c r="F23" s="12">
-        <f t="shared" si="3"/>
-        <v>5.8246000000000001E-3</v>
-      </c>
-      <c r="G23" s="14">
-        <f t="shared" ref="G23:G25" si="4">F23/F$23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="str">
-        <f t="shared" ref="B24:B34" si="5">B3</f>
-        <v>split_vec_linear</v>
-      </c>
-      <c r="C24" s="2">
-        <f t="shared" si="2"/>
-        <v>1024</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="2"/>
-        <v>1.1573E-3</v>
-      </c>
-      <c r="E24" s="5">
-        <f t="shared" ref="E24:E25" si="6">D24/D$23</f>
-        <v>0.83601820414650008</v>
-      </c>
-      <c r="F24" s="4">
-        <f t="shared" si="3"/>
-        <v>5.9960999999999999E-3</v>
-      </c>
-      <c r="G24" s="16">
-        <f t="shared" si="4"/>
-        <v>1.029444081997047</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v>split_vec_doubling</v>
-      </c>
-      <c r="C25" s="18">
-        <f t="shared" si="2"/>
-        <v>1024</v>
-      </c>
-      <c r="D25" s="19">
-        <f t="shared" si="2"/>
-        <v>1.1984999999999999E-3</v>
-      </c>
-      <c r="E25" s="20">
-        <f t="shared" si="6"/>
-        <v>0.86578053890052731</v>
-      </c>
-      <c r="F25" s="19">
-        <f t="shared" si="3"/>
-        <v>6.0682000000000002E-3</v>
-      </c>
-      <c r="G25" s="21">
-        <f t="shared" si="4"/>
-        <v>1.0418226144284586</v>
-      </c>
-      <c r="L25">
-        <f>D25/D23</f>
-        <v>0.86578053890052731</v>
-      </c>
-      <c r="N25">
-        <f>F25/F23</f>
-        <v>1.0418226144284586</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="str">
-        <f t="shared" si="5"/>
-        <v>std_vec</v>
-      </c>
-      <c r="C26" s="11">
-        <f t="shared" si="2"/>
-        <v>16384</v>
-      </c>
-      <c r="D26" s="12">
-        <f t="shared" si="2"/>
-        <v>2.2847000000000003E-2</v>
-      </c>
-      <c r="E26" s="13">
+      <c r="E26" s="11">
         <f>D26/D$26</f>
         <v>1</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="10">
+        <f>F2</f>
+        <v>5.8246000000000001E-3</v>
+      </c>
+      <c r="G26" s="12">
+        <f t="shared" ref="G26:G29" si="2">F26/F$26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="13" t="str">
+        <f>B3</f>
+        <v>split_vec_linear</v>
+      </c>
+      <c r="C27" s="2">
+        <f>C3</f>
+        <v>1024</v>
+      </c>
+      <c r="D27" s="4">
+        <f>D3</f>
+        <v>1.1573E-3</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" ref="E27:E29" si="3">D27/D$26</f>
+        <v>0.83601820414650008</v>
+      </c>
+      <c r="F27" s="4">
+        <f>F3</f>
+        <v>5.9960999999999999E-3</v>
+      </c>
+      <c r="G27" s="14">
+        <f t="shared" si="2"/>
+        <v>1.029444081997047</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="13" t="str">
+        <f t="shared" ref="B28:D41" si="4">B4</f>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="4"/>
+        <v>1024</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="4"/>
+        <v>1.1984999999999999E-3</v>
+      </c>
+      <c r="E28" s="5">
         <f t="shared" si="3"/>
+        <v>0.86578053890052731</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" ref="F28:F41" si="5">F4</f>
+        <v>6.0682000000000002E-3</v>
+      </c>
+      <c r="G28" s="14">
+        <f t="shared" si="2"/>
+        <v>1.0418226144284586</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C29" s="16">
+        <f t="shared" si="4"/>
+        <v>1024</v>
+      </c>
+      <c r="D29" s="17">
+        <f t="shared" si="4"/>
+        <v>1.1973999999999999E-3</v>
+      </c>
+      <c r="E29" s="18">
+        <f t="shared" si="3"/>
+        <v>0.86498591345806541</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" si="5"/>
+        <v>6.0742000000000001E-3</v>
+      </c>
+      <c r="G29" s="19">
+        <f t="shared" si="2"/>
+        <v>1.042852728084332</v>
+      </c>
+      <c r="L29">
+        <f>D29/D26</f>
+        <v>0.86498591345806541</v>
+      </c>
+      <c r="N29">
+        <f>F29/F26</f>
+        <v>1.042852728084332</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>std_vec</v>
+      </c>
+      <c r="C30" s="9">
+        <f t="shared" si="4"/>
+        <v>16384</v>
+      </c>
+      <c r="D30" s="10">
+        <f t="shared" si="4"/>
+        <v>2.2847000000000003E-2</v>
+      </c>
+      <c r="E30" s="11">
+        <f>D30/D$30</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="5"/>
         <v>0.10091</v>
       </c>
-      <c r="G26" s="14">
-        <f>F26/F$26</f>
+      <c r="G30" s="12">
+        <f>F30/F$30</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="str">
+    <row r="31" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>split_vec_linear</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="4"/>
+        <v>16384</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="4"/>
+        <v>1.9015000000000001E-2</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" ref="E31:G33" si="6">D31/D$30</f>
+        <v>0.83227557228520144</v>
+      </c>
+      <c r="F31" s="4">
         <f t="shared" si="5"/>
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="G31" s="20">
+        <f t="shared" si="6"/>
+        <v>1.0157566148052719</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="4"/>
+        <v>16384</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="4"/>
+        <v>1.9E-2</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="6"/>
+        <v>0.83161903094498169</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" si="5"/>
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="G32" s="20">
+        <f t="shared" si="6"/>
+        <v>1.0157566148052719</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C33" s="16">
+        <f t="shared" si="4"/>
+        <v>16384</v>
+      </c>
+      <c r="D33" s="17">
+        <f t="shared" si="4"/>
+        <v>1.9010000000000003E-2</v>
+      </c>
+      <c r="E33" s="18">
+        <f t="shared" si="6"/>
+        <v>0.83205672517179496</v>
+      </c>
+      <c r="F33" s="17">
+        <f t="shared" si="5"/>
+        <v>0.10340000000000001</v>
+      </c>
+      <c r="G33" s="21">
+        <f t="shared" si="6"/>
+        <v>1.0246754533742939</v>
+      </c>
+      <c r="L33">
+        <f>D33/D30</f>
+        <v>0.83205672517179496</v>
+      </c>
+      <c r="N33">
+        <f>F33/F30</f>
+        <v>1.0246754533742939</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>std_vec</v>
+      </c>
+      <c r="C34" s="9">
+        <f t="shared" si="4"/>
+        <v>262144</v>
+      </c>
+      <c r="D34" s="10">
+        <f t="shared" si="4"/>
+        <v>0.36402999999999996</v>
+      </c>
+      <c r="E34" s="11">
+        <f>D34/D$34</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="10">
+        <f t="shared" si="5"/>
+        <v>2.4842</v>
+      </c>
+      <c r="G34" s="12">
+        <f>F34/F$34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="str">
+        <f t="shared" si="4"/>
         <v>split_vec_linear</v>
       </c>
-      <c r="C27" s="2">
-        <f t="shared" si="2"/>
-        <v>16384</v>
-      </c>
-      <c r="D27" s="4">
-        <f t="shared" si="2"/>
-        <v>1.9015000000000001E-2</v>
-      </c>
-      <c r="E27" s="5">
-        <f t="shared" ref="E27:G28" si="7">D27/D$26</f>
-        <v>0.83227557228520144</v>
-      </c>
-      <c r="F27" s="4">
-        <f t="shared" si="3"/>
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="G27" s="22">
+      <c r="C35" s="2">
+        <f t="shared" si="4"/>
+        <v>262144</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="4"/>
+        <v>0.31098999999999999</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" ref="E35:G37" si="7">D35/D$34</f>
+        <v>0.85429772271516091</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" si="5"/>
+        <v>2.5592999999999999</v>
+      </c>
+      <c r="G35" s="20">
         <f t="shared" si="7"/>
-        <v>1.0157566148052719</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="17" t="str">
+        <v>1.0302310603011029</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="4"/>
+        <v>262144</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="4"/>
+        <v>0.30449999999999999</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="7"/>
+        <v>0.83646952174271361</v>
+      </c>
+      <c r="F36" s="4">
         <f t="shared" si="5"/>
+        <v>2.5009000000000001</v>
+      </c>
+      <c r="G36" s="20">
+        <f t="shared" si="7"/>
+        <v>1.0067224861122293</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C37" s="16">
+        <f t="shared" si="4"/>
+        <v>262144</v>
+      </c>
+      <c r="D37" s="17">
+        <f t="shared" si="4"/>
+        <v>0.30580000000000002</v>
+      </c>
+      <c r="E37" s="18">
+        <f t="shared" si="7"/>
+        <v>0.84004065598989108</v>
+      </c>
+      <c r="F37" s="17">
+        <f t="shared" si="5"/>
+        <v>2.5104000000000002</v>
+      </c>
+      <c r="G37" s="21">
+        <f t="shared" si="7"/>
+        <v>1.0105466548587072</v>
+      </c>
+      <c r="L37">
+        <f>D37/D34</f>
+        <v>0.84004065598989108</v>
+      </c>
+      <c r="N37">
+        <f>F37/F34</f>
+        <v>1.0105466548587072</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>std_vec</v>
+      </c>
+      <c r="C38" s="9">
+        <f t="shared" si="4"/>
+        <v>4194304</v>
+      </c>
+      <c r="D38" s="10">
+        <f t="shared" si="4"/>
+        <v>6.6346999999999996</v>
+      </c>
+      <c r="E38" s="11">
+        <f>D38/D$38</f>
+        <v>1</v>
+      </c>
+      <c r="F38" s="10">
+        <f t="shared" si="5"/>
+        <v>39.786999999999999</v>
+      </c>
+      <c r="G38" s="12">
+        <f>F38/F$38</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B39" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>split_vec_linear</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="4"/>
+        <v>4194304</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="4"/>
+        <v>5.8848000000000003</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" ref="E39:G41" si="8">D39/D$38</f>
+        <v>0.88697303570621133</v>
+      </c>
+      <c r="F39" s="4">
+        <f t="shared" si="5"/>
+        <v>40.158000000000001</v>
+      </c>
+      <c r="G39" s="20">
+        <f t="shared" si="8"/>
+        <v>1.009324653781386</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" s="13" t="str">
+        <f t="shared" si="4"/>
         <v>split_vec_doubling</v>
       </c>
-      <c r="C28" s="18">
-        <f t="shared" si="2"/>
-        <v>16384</v>
-      </c>
-      <c r="D28" s="19">
-        <f t="shared" si="2"/>
-        <v>1.9E-2</v>
-      </c>
-      <c r="E28" s="20">
-        <f t="shared" si="7"/>
-        <v>0.83161903094498169</v>
-      </c>
-      <c r="F28" s="19">
-        <f t="shared" si="3"/>
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="G28" s="23">
-        <f t="shared" si="7"/>
-        <v>1.0157566148052719</v>
-      </c>
-      <c r="L28">
-        <f>D28/D26</f>
-        <v>0.83161903094498169</v>
-      </c>
-      <c r="N28">
-        <f>F28/F26</f>
-        <v>1.0157566148052719</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="str">
+      <c r="C40" s="2">
+        <f t="shared" si="4"/>
+        <v>4194304</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="4"/>
+        <v>5.6269999999999998</v>
+      </c>
+      <c r="E40" s="5">
+        <f t="shared" si="8"/>
+        <v>0.84811671967082158</v>
+      </c>
+      <c r="F40" s="4">
         <f t="shared" si="5"/>
-        <v>std_vec</v>
-      </c>
-      <c r="C29" s="11">
-        <f t="shared" si="2"/>
-        <v>262144</v>
-      </c>
-      <c r="D29" s="12">
-        <f t="shared" si="2"/>
-        <v>0.36402999999999996</v>
-      </c>
-      <c r="E29" s="13">
-        <f>D29/D$29</f>
-        <v>1</v>
-      </c>
-      <c r="F29" s="12">
-        <f t="shared" si="3"/>
-        <v>2.4842</v>
-      </c>
-      <c r="G29" s="14">
-        <f>F29/F$29</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="15" t="str">
+        <v>40.21</v>
+      </c>
+      <c r="G40" s="20">
+        <f t="shared" si="8"/>
+        <v>1.0106316133410411</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C41" s="16">
+        <f t="shared" si="4"/>
+        <v>4194304</v>
+      </c>
+      <c r="D41" s="17">
+        <f t="shared" si="4"/>
+        <v>5.6340000000000003</v>
+      </c>
+      <c r="E41" s="18">
+        <f t="shared" si="8"/>
+        <v>0.84917177867876481</v>
+      </c>
+      <c r="F41" s="17">
         <f t="shared" si="5"/>
-        <v>split_vec_linear</v>
-      </c>
-      <c r="C30" s="2">
-        <f t="shared" si="2"/>
-        <v>262144</v>
-      </c>
-      <c r="D30" s="4">
-        <f t="shared" si="2"/>
-        <v>0.31098999999999999</v>
-      </c>
-      <c r="E30" s="5">
-        <f t="shared" ref="E30:G31" si="8">D30/D$29</f>
-        <v>0.85429772271516091</v>
-      </c>
-      <c r="F30" s="4">
-        <f t="shared" si="3"/>
-        <v>2.5592999999999999</v>
-      </c>
-      <c r="G30" s="22">
+        <v>40.17</v>
+      </c>
+      <c r="G41" s="21">
         <f t="shared" si="8"/>
-        <v>1.0302310603011029</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v>split_vec_doubling</v>
-      </c>
-      <c r="C31" s="18">
-        <f t="shared" si="2"/>
-        <v>262144</v>
-      </c>
-      <c r="D31" s="19">
-        <f t="shared" si="2"/>
-        <v>0.30449999999999999</v>
-      </c>
-      <c r="E31" s="20">
-        <f t="shared" si="8"/>
-        <v>0.83646952174271361</v>
-      </c>
-      <c r="F31" s="19">
-        <f t="shared" si="3"/>
-        <v>2.5009000000000001</v>
-      </c>
-      <c r="G31" s="23">
-        <f t="shared" si="8"/>
-        <v>1.0067224861122293</v>
-      </c>
-      <c r="L31">
-        <f>D31/D29</f>
-        <v>0.83646952174271361</v>
-      </c>
-      <c r="N31">
-        <f>F31/F29</f>
-        <v>1.0067224861122293</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="str">
-        <f t="shared" si="5"/>
-        <v>std_vec</v>
-      </c>
-      <c r="C32" s="11">
-        <f t="shared" si="2"/>
-        <v>4194304</v>
-      </c>
-      <c r="D32" s="12">
-        <f t="shared" si="2"/>
-        <v>6.6346999999999996</v>
-      </c>
-      <c r="E32" s="13">
-        <f>D32/D$32</f>
-        <v>1</v>
-      </c>
-      <c r="F32" s="12">
-        <f t="shared" si="3"/>
-        <v>39.786999999999999</v>
-      </c>
-      <c r="G32" s="14">
-        <f>F32/F$32</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="15" t="str">
-        <f t="shared" si="5"/>
-        <v>split_vec_linear</v>
-      </c>
-      <c r="C33" s="2">
-        <f t="shared" si="2"/>
-        <v>4194304</v>
-      </c>
-      <c r="D33" s="4">
-        <f t="shared" si="2"/>
-        <v>5.8848000000000003</v>
-      </c>
-      <c r="E33" s="5">
-        <f t="shared" ref="E33:G34" si="9">D33/D$32</f>
-        <v>0.88697303570621133</v>
-      </c>
-      <c r="F33" s="4">
-        <f t="shared" si="3"/>
-        <v>40.158000000000001</v>
-      </c>
-      <c r="G33" s="22">
-        <f t="shared" si="9"/>
-        <v>1.009324653781386</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v>split_vec_doubling</v>
-      </c>
-      <c r="C34" s="18">
-        <f t="shared" si="2"/>
-        <v>4194304</v>
-      </c>
-      <c r="D34" s="19">
-        <f t="shared" si="2"/>
-        <v>5.6269999999999998</v>
-      </c>
-      <c r="E34" s="20">
-        <f t="shared" si="9"/>
-        <v>0.84811671967082158</v>
-      </c>
-      <c r="F34" s="19">
-        <f t="shared" si="3"/>
-        <v>40.21</v>
-      </c>
-      <c r="G34" s="23">
-        <f t="shared" si="9"/>
-        <v>1.0106316133410411</v>
-      </c>
-      <c r="L34">
-        <f>D34/D32</f>
-        <v>0.84811671967082158</v>
-      </c>
-      <c r="N34">
-        <f>F34/F32</f>
-        <v>1.0106316133410411</v>
+        <v>1.0096262598336141</v>
+      </c>
+      <c r="L41">
+        <f>D41/D38</f>
+        <v>0.84917177867876481</v>
+      </c>
+      <c r="N41">
+        <f>F41/F38</f>
+        <v>1.0096262598336141</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
   </mergeCells>
-  <conditionalFormatting sqref="E23:E34 G23:G34">
+  <conditionalFormatting sqref="E26:E41 G26:G41">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -2186,7 +2576,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E23:E34 G23:G34</xm:sqref>
+          <xm:sqref>E26:E41 G26:G41</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2196,10 +2586,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7FC78D-902C-4DF1-8F50-38A3D8921053}">
-  <dimension ref="B1:N34"/>
+  <dimension ref="B1:N44"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +2623,7 @@
         <v>1.1594999999999999E-3</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F7" si="0">J2/1000</f>
+        <f t="shared" ref="F2:F9" si="0">J2/1000</f>
         <v>6.2013999999999993E-3</v>
       </c>
       <c r="H2">
@@ -2251,18 +2641,18 @@
         <v>1024</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D7" si="1">H3/1000</f>
+        <f t="shared" ref="D3:D9" si="1">H3/1000</f>
         <v>3.0141E-3</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>8.3306000000000005E-3</v>
+        <v>8.147999999999999E-3</v>
       </c>
       <c r="H3">
         <v>3.0141</v>
       </c>
       <c r="J3">
-        <v>8.3306000000000004</v>
+        <v>8.1479999999999997</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -2274,14 +2664,14 @@
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>1.6335E-3</v>
+        <v>1.6156E-3</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>6.6529999999999992E-3</v>
       </c>
       <c r="H4">
-        <v>1.6335</v>
+        <v>1.6155999999999999</v>
       </c>
       <c r="J4">
         <v>6.6529999999999996</v>
@@ -2289,526 +2679,708 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>16384</v>
+        <v>1024</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>1.8957000000000002E-2</v>
+        <v>6.1809999999999999E-3</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0.15561000000000003</v>
+        <v>8.4968000000000005E-3</v>
       </c>
       <c r="H5">
-        <v>18.957000000000001</v>
+        <v>6.181</v>
       </c>
       <c r="J5">
-        <v>155.61000000000001</v>
+        <v>8.4968000000000004</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>16384</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>4.9530999999999999E-2</v>
+        <v>2.2178999999999997E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0.17565999999999998</v>
+        <v>0.15561000000000003</v>
       </c>
       <c r="H6">
-        <v>49.530999999999999</v>
+        <v>22.178999999999998</v>
       </c>
       <c r="J6">
-        <v>175.66</v>
+        <v>155.61000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>16384</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>2.8513E-2</v>
+        <v>5.5296999999999999E-2</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0.15762999999999999</v>
+        <v>0.17155000000000001</v>
       </c>
       <c r="H7">
-        <v>28.513000000000002</v>
+        <v>55.296999999999997</v>
       </c>
       <c r="J7">
-        <v>157.63</v>
+        <v>171.55</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>16384</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>2.8513E-2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.15762999999999999</v>
+      </c>
+      <c r="H8">
+        <v>28.513000000000002</v>
+      </c>
+      <c r="J8">
+        <v>157.63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>16384</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.15816</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.23221</v>
+      </c>
+      <c r="H9">
+        <v>158.16</v>
+      </c>
+      <c r="J9">
+        <v>232.21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C10">
         <v>262144</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <f>540.66/1000</f>
         <v>0.54065999999999992</v>
       </c>
-      <c r="F8">
+      <c r="F10">
         <v>10.193</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>262144</v>
-      </c>
-      <c r="D9">
-        <v>1.0773999999999999</v>
-      </c>
-      <c r="F9">
-        <v>11.03</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>262144</v>
-      </c>
-      <c r="D10">
-        <f>703.37/1000</f>
-        <v>0.70337000000000005</v>
-      </c>
-      <c r="F10">
-        <v>10.824</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>4194304</v>
+        <v>262144</v>
       </c>
       <c r="D11">
-        <v>41.655000000000001</v>
+        <v>1.0773999999999999</v>
       </c>
       <c r="F11">
-        <v>253.34</v>
+        <v>11.03</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>4194304</v>
+        <v>262144</v>
       </c>
       <c r="D12">
-        <v>69.358000000000004</v>
+        <f>674.98/1000</f>
+        <v>0.67498000000000002</v>
       </c>
       <c r="F12">
-        <v>267.49</v>
+        <v>10.824</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>262144</v>
+      </c>
+      <c r="D13">
+        <v>3.4293</v>
+      </c>
+      <c r="F13">
+        <v>16.074999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>4194304</v>
+      </c>
+      <c r="D14">
+        <v>46.395000000000003</v>
+      </c>
+      <c r="F14">
+        <v>253.34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>4194304</v>
+      </c>
+      <c r="D15">
+        <v>69.316000000000003</v>
+      </c>
+      <c r="F15">
+        <v>267.49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="C13">
+      <c r="C16">
         <v>4194304</v>
       </c>
-      <c r="D13">
+      <c r="D16">
         <v>51.656999999999996</v>
       </c>
-      <c r="F13">
+      <c r="F16">
         <v>236.89</v>
       </c>
     </row>
-    <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>4194304</v>
+      </c>
+      <c r="D17">
+        <v>188.15</v>
+      </c>
+      <c r="F17">
+        <v>332.54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="7" t="str">
-        <f t="shared" ref="C22:C34" si="2">C1</f>
+      <c r="C25" s="7" t="str">
+        <f>C1</f>
         <v>number of elements</v>
       </c>
-      <c r="D22" s="8" t="str">
-        <f t="shared" ref="D22:D34" si="3">D1</f>
+      <c r="D25" s="35" t="str">
+        <f>D1</f>
         <v>u64 x 1</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8" t="str">
-        <f t="shared" ref="F22:F34" si="4">F1</f>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35" t="str">
+        <f>F1</f>
         <v>u64 x 16</v>
       </c>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="str">
+      <c r="G25" s="36"/>
+    </row>
+    <row r="26" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="str">
         <f>B2</f>
         <v>std_vec</v>
       </c>
-      <c r="C23" s="11">
-        <f t="shared" si="2"/>
+      <c r="C26" s="9">
+        <f>C2</f>
         <v>1024</v>
       </c>
-      <c r="D23" s="12">
-        <f t="shared" si="3"/>
+      <c r="D26" s="10">
+        <f>D2</f>
         <v>1.1594999999999999E-3</v>
       </c>
-      <c r="E23" s="13">
-        <f>D23/D$23</f>
-        <v>1</v>
-      </c>
-      <c r="F23" s="12">
-        <f t="shared" si="4"/>
-        <v>6.2013999999999993E-3</v>
-      </c>
-      <c r="G23" s="14">
-        <f t="shared" ref="G23:G25" si="5">F23/F$23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="str">
-        <f t="shared" ref="B24:B34" si="6">B3</f>
-        <v>split_vec_linear</v>
-      </c>
-      <c r="C24" s="2">
-        <f t="shared" si="2"/>
-        <v>1024</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="3"/>
-        <v>3.0141E-3</v>
-      </c>
-      <c r="E24" s="5">
-        <f t="shared" ref="E24:E25" si="7">D24/D$23</f>
-        <v>2.5994825355756794</v>
-      </c>
-      <c r="F24" s="4">
-        <f t="shared" si="4"/>
-        <v>8.3306000000000005E-3</v>
-      </c>
-      <c r="G24" s="16">
-        <f t="shared" si="5"/>
-        <v>1.3433418260392818</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v>split_vec_doubling</v>
-      </c>
-      <c r="C25" s="18">
-        <f t="shared" si="2"/>
-        <v>1024</v>
-      </c>
-      <c r="D25" s="19">
-        <f t="shared" si="3"/>
-        <v>1.6335E-3</v>
-      </c>
-      <c r="E25" s="20">
-        <f t="shared" si="7"/>
-        <v>1.4087968952134542</v>
-      </c>
-      <c r="F25" s="19">
-        <f t="shared" si="4"/>
-        <v>6.6529999999999992E-3</v>
-      </c>
-      <c r="G25" s="21">
-        <f t="shared" si="5"/>
-        <v>1.0728222659399491</v>
-      </c>
-      <c r="L25">
-        <f>D25/D23</f>
-        <v>1.4087968952134542</v>
-      </c>
-      <c r="N25">
-        <f>F25/F23</f>
-        <v>1.0728222659399491</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="str">
-        <f t="shared" si="6"/>
-        <v>std_vec</v>
-      </c>
-      <c r="C26" s="11">
-        <f t="shared" si="2"/>
-        <v>16384</v>
-      </c>
-      <c r="D26" s="12">
-        <f t="shared" si="3"/>
-        <v>1.8957000000000002E-2</v>
-      </c>
-      <c r="E26" s="13">
+      <c r="E26" s="11">
         <f>D26/D$26</f>
         <v>1</v>
       </c>
-      <c r="F26" s="12">
-        <f t="shared" si="4"/>
+      <c r="F26" s="10">
+        <f>F2</f>
+        <v>6.2013999999999993E-3</v>
+      </c>
+      <c r="G26" s="12">
+        <f t="shared" ref="G26:G29" si="2">F26/F$26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="13" t="str">
+        <f t="shared" ref="B27:B41" si="3">B3</f>
+        <v>split_vec_linear</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" ref="B27:D27" si="4">C3</f>
+        <v>1024</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="4"/>
+        <v>3.0141E-3</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" ref="E27:E29" si="5">D27/D$26</f>
+        <v>2.5994825355756794</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" ref="F27:F41" si="6">F3</f>
+        <v>8.147999999999999E-3</v>
+      </c>
+      <c r="G27" s="14">
+        <f t="shared" si="2"/>
+        <v>1.3138968619989035</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" ref="C28:D41" si="7">C4</f>
+        <v>1024</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="7"/>
+        <v>1.6156E-3</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="5"/>
+        <v>1.3933592065545495</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="6"/>
+        <v>6.6529999999999992E-3</v>
+      </c>
+      <c r="G28" s="14">
+        <f t="shared" si="2"/>
+        <v>1.0728222659399491</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C29" s="16">
+        <f t="shared" si="7"/>
+        <v>1024</v>
+      </c>
+      <c r="D29" s="17">
+        <f t="shared" si="7"/>
+        <v>6.1809999999999999E-3</v>
+      </c>
+      <c r="E29" s="18">
+        <f t="shared" si="5"/>
+        <v>5.3307460112117298</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" si="6"/>
+        <v>8.4968000000000005E-3</v>
+      </c>
+      <c r="G29" s="19">
+        <f t="shared" si="2"/>
+        <v>1.3701422259489795</v>
+      </c>
+      <c r="L29">
+        <f>D29/D26</f>
+        <v>5.3307460112117298</v>
+      </c>
+      <c r="N29">
+        <f>F29/F26</f>
+        <v>1.3701422259489795</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>std_vec</v>
+      </c>
+      <c r="C30" s="9">
+        <f t="shared" si="7"/>
+        <v>16384</v>
+      </c>
+      <c r="D30" s="10">
+        <f t="shared" si="7"/>
+        <v>2.2178999999999997E-2</v>
+      </c>
+      <c r="E30" s="11">
+        <f>D30/D$30</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="6"/>
         <v>0.15561000000000003</v>
       </c>
-      <c r="G26" s="14">
-        <f>F26/F$26</f>
+      <c r="G30" s="12">
+        <f>F30/F$30</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="str">
+    <row r="31" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>split_vec_linear</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="7"/>
+        <v>16384</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="7"/>
+        <v>5.5296999999999999E-2</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" ref="E31:E33" si="8">D31/D$30</f>
+        <v>2.4932143018170345</v>
+      </c>
+      <c r="F31" s="4">
         <f t="shared" si="6"/>
+        <v>0.17155000000000001</v>
+      </c>
+      <c r="G31" s="20">
+        <f t="shared" ref="G31:G33" si="9">F31/F$30</f>
+        <v>1.1024355761197866</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="7"/>
+        <v>16384</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="7"/>
+        <v>2.8513E-2</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="8"/>
+        <v>1.285585463726949</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" si="6"/>
+        <v>0.15762999999999999</v>
+      </c>
+      <c r="G32" s="20">
+        <f t="shared" si="9"/>
+        <v>1.0129811708759076</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C33" s="16">
+        <f t="shared" si="7"/>
+        <v>16384</v>
+      </c>
+      <c r="D33" s="17">
+        <f t="shared" si="7"/>
+        <v>0.15816</v>
+      </c>
+      <c r="E33" s="18">
+        <f t="shared" si="8"/>
+        <v>7.1310699310158263</v>
+      </c>
+      <c r="F33" s="17">
+        <f t="shared" si="6"/>
+        <v>0.23221</v>
+      </c>
+      <c r="G33" s="21">
+        <f t="shared" si="9"/>
+        <v>1.4922562817299656</v>
+      </c>
+      <c r="L33">
+        <f>D33/D30</f>
+        <v>7.1310699310158263</v>
+      </c>
+      <c r="N33">
+        <f>F33/F30</f>
+        <v>1.4922562817299656</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>std_vec</v>
+      </c>
+      <c r="C34" s="9">
+        <f t="shared" si="7"/>
+        <v>262144</v>
+      </c>
+      <c r="D34" s="10">
+        <f t="shared" si="7"/>
+        <v>0.54065999999999992</v>
+      </c>
+      <c r="E34" s="11">
+        <f>D34/D$34</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="10">
+        <f t="shared" si="6"/>
+        <v>10.193</v>
+      </c>
+      <c r="G34" s="12">
+        <f>F34/F$34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="str">
+        <f t="shared" si="3"/>
         <v>split_vec_linear</v>
       </c>
-      <c r="C27" s="2">
-        <f t="shared" si="2"/>
-        <v>16384</v>
-      </c>
-      <c r="D27" s="4">
+      <c r="C35" s="2">
+        <f t="shared" si="7"/>
+        <v>262144</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="7"/>
+        <v>1.0773999999999999</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" ref="E35:E37" si="10">D35/D$34</f>
+        <v>1.9927496023378835</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" si="6"/>
+        <v>11.03</v>
+      </c>
+      <c r="G35" s="20">
+        <f t="shared" ref="G35:G37" si="11">F35/F$34</f>
+        <v>1.0821151770823114</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>4.9530999999999999E-2</v>
-      </c>
-      <c r="E27" s="5">
-        <f t="shared" ref="E27:G28" si="8">D27/D$26</f>
-        <v>2.6128079337447905</v>
-      </c>
-      <c r="F27" s="4">
-        <f t="shared" si="4"/>
-        <v>0.17565999999999998</v>
-      </c>
-      <c r="G27" s="22">
-        <f t="shared" si="8"/>
-        <v>1.1288477604267075</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="17" t="str">
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="7"/>
+        <v>262144</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="7"/>
+        <v>0.67498000000000002</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="10"/>
+        <v>1.2484370954019164</v>
+      </c>
+      <c r="F36" s="4">
         <f t="shared" si="6"/>
+        <v>10.824</v>
+      </c>
+      <c r="G36" s="20">
+        <f t="shared" si="11"/>
+        <v>1.0619052290787796</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C37" s="16">
+        <f t="shared" si="7"/>
+        <v>262144</v>
+      </c>
+      <c r="D37" s="17">
+        <f t="shared" si="7"/>
+        <v>3.4293</v>
+      </c>
+      <c r="E37" s="18">
+        <f t="shared" si="10"/>
+        <v>6.3428032404838541</v>
+      </c>
+      <c r="F37" s="17">
+        <f t="shared" si="6"/>
+        <v>16.074999999999999</v>
+      </c>
+      <c r="G37" s="21">
+        <f t="shared" si="11"/>
+        <v>1.5770626900814284</v>
+      </c>
+      <c r="L37">
+        <f>D37/D34</f>
+        <v>6.3428032404838541</v>
+      </c>
+      <c r="N37">
+        <f>F37/F34</f>
+        <v>1.5770626900814284</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>std_vec</v>
+      </c>
+      <c r="C38" s="9">
+        <f t="shared" si="7"/>
+        <v>4194304</v>
+      </c>
+      <c r="D38" s="10">
+        <f t="shared" si="7"/>
+        <v>46.395000000000003</v>
+      </c>
+      <c r="E38" s="11">
+        <f>D38/D$38</f>
+        <v>1</v>
+      </c>
+      <c r="F38" s="10">
+        <f t="shared" si="6"/>
+        <v>253.34</v>
+      </c>
+      <c r="G38" s="12">
+        <f>F38/F$38</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>split_vec_linear</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="7"/>
+        <v>4194304</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="7"/>
+        <v>69.316000000000003</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" ref="E39:E41" si="12">D39/D$38</f>
+        <v>1.4940403060674641</v>
+      </c>
+      <c r="F39" s="4">
+        <f t="shared" si="6"/>
+        <v>267.49</v>
+      </c>
+      <c r="G39" s="20">
+        <f t="shared" ref="G39:G41" si="13">F39/F$38</f>
+        <v>1.0558537933212284</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="13" t="str">
+        <f t="shared" si="3"/>
         <v>split_vec_doubling</v>
       </c>
-      <c r="C28" s="18">
-        <f t="shared" si="2"/>
-        <v>16384</v>
-      </c>
-      <c r="D28" s="19">
+      <c r="C40" s="2">
+        <f t="shared" si="7"/>
+        <v>4194304</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="7"/>
+        <v>51.656999999999996</v>
+      </c>
+      <c r="E40" s="5">
+        <f t="shared" si="12"/>
+        <v>1.113417394115745</v>
+      </c>
+      <c r="F40" s="4">
+        <f t="shared" si="6"/>
+        <v>236.89</v>
+      </c>
+      <c r="G40" s="20">
+        <f t="shared" si="13"/>
+        <v>0.93506749822373092</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>2.8513E-2</v>
-      </c>
-      <c r="E28" s="20">
-        <f t="shared" si="8"/>
-        <v>1.5040881996096427</v>
-      </c>
-      <c r="F28" s="19">
-        <f t="shared" si="4"/>
-        <v>0.15762999999999999</v>
-      </c>
-      <c r="G28" s="23">
-        <f t="shared" si="8"/>
-        <v>1.0129811708759076</v>
-      </c>
-      <c r="L28">
-        <f>D28/D26</f>
-        <v>1.5040881996096427</v>
-      </c>
-      <c r="N28">
-        <f>F28/F26</f>
-        <v>1.0129811708759076</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="str">
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C41" s="16">
+        <f t="shared" si="7"/>
+        <v>4194304</v>
+      </c>
+      <c r="D41" s="17">
+        <f t="shared" si="7"/>
+        <v>188.15</v>
+      </c>
+      <c r="E41" s="18">
+        <f t="shared" si="12"/>
+        <v>4.0553939002047636</v>
+      </c>
+      <c r="F41" s="17">
         <f t="shared" si="6"/>
-        <v>std_vec</v>
-      </c>
-      <c r="C29" s="11">
-        <f t="shared" si="2"/>
-        <v>262144</v>
-      </c>
-      <c r="D29" s="12">
-        <f t="shared" si="3"/>
-        <v>0.54065999999999992</v>
-      </c>
-      <c r="E29" s="13">
-        <f>D29/D$29</f>
-        <v>1</v>
-      </c>
-      <c r="F29" s="12">
-        <f t="shared" si="4"/>
-        <v>10.193</v>
-      </c>
-      <c r="G29" s="14">
-        <f>F29/F$29</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>split_vec_linear</v>
-      </c>
-      <c r="C30" s="2">
-        <f t="shared" si="2"/>
-        <v>262144</v>
-      </c>
-      <c r="D30" s="4">
-        <f t="shared" si="3"/>
-        <v>1.0773999999999999</v>
-      </c>
-      <c r="E30" s="5">
-        <f t="shared" ref="E30:G31" si="9">D30/D$29</f>
-        <v>1.9927496023378835</v>
-      </c>
-      <c r="F30" s="4">
-        <f t="shared" si="4"/>
-        <v>11.03</v>
-      </c>
-      <c r="G30" s="22">
-        <f t="shared" si="9"/>
-        <v>1.0821151770823114</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v>split_vec_doubling</v>
-      </c>
-      <c r="C31" s="18">
-        <f t="shared" si="2"/>
-        <v>262144</v>
-      </c>
-      <c r="D31" s="19">
-        <f t="shared" si="3"/>
-        <v>0.70337000000000005</v>
-      </c>
-      <c r="E31" s="20">
-        <f t="shared" si="9"/>
-        <v>1.3009469907150522</v>
-      </c>
-      <c r="F31" s="19">
-        <f t="shared" si="4"/>
-        <v>10.824</v>
-      </c>
-      <c r="G31" s="23">
-        <f t="shared" si="9"/>
-        <v>1.0619052290787796</v>
-      </c>
-      <c r="L31">
-        <f>D31/D29</f>
-        <v>1.3009469907150522</v>
-      </c>
-      <c r="N31">
-        <f>F31/F29</f>
-        <v>1.0619052290787796</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="str">
-        <f t="shared" si="6"/>
-        <v>std_vec</v>
-      </c>
-      <c r="C32" s="11">
-        <f t="shared" si="2"/>
-        <v>4194304</v>
-      </c>
-      <c r="D32" s="12">
-        <f t="shared" si="3"/>
-        <v>41.655000000000001</v>
-      </c>
-      <c r="E32" s="13">
-        <f>D32/D$32</f>
-        <v>1</v>
-      </c>
-      <c r="F32" s="12">
-        <f t="shared" si="4"/>
-        <v>253.34</v>
-      </c>
-      <c r="G32" s="14">
-        <f>F32/F$32</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="15" t="str">
-        <f t="shared" si="6"/>
-        <v>split_vec_linear</v>
-      </c>
-      <c r="C33" s="2">
-        <f t="shared" si="2"/>
-        <v>4194304</v>
-      </c>
-      <c r="D33" s="4">
-        <f t="shared" si="3"/>
-        <v>69.358000000000004</v>
-      </c>
-      <c r="E33" s="5">
-        <f t="shared" ref="E33:G34" si="10">D33/D$32</f>
-        <v>1.6650582163005643</v>
-      </c>
-      <c r="F33" s="4">
-        <f t="shared" si="4"/>
-        <v>267.49</v>
-      </c>
-      <c r="G33" s="22">
-        <f t="shared" si="10"/>
-        <v>1.0558537933212284</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v>split_vec_doubling</v>
-      </c>
-      <c r="C34" s="18">
-        <f t="shared" si="2"/>
-        <v>4194304</v>
-      </c>
-      <c r="D34" s="19">
-        <f t="shared" si="3"/>
-        <v>51.656999999999996</v>
-      </c>
-      <c r="E34" s="20">
-        <f t="shared" si="10"/>
-        <v>1.2401152322650342</v>
-      </c>
-      <c r="F34" s="19">
-        <f t="shared" si="4"/>
-        <v>236.89</v>
-      </c>
-      <c r="G34" s="23">
-        <f t="shared" si="10"/>
-        <v>0.93506749822373092</v>
-      </c>
-      <c r="L34">
-        <f>D34/D32</f>
-        <v>1.2401152322650342</v>
-      </c>
-      <c r="N34">
-        <f>F34/F32</f>
-        <v>0.93506749822373092</v>
+        <v>332.54</v>
+      </c>
+      <c r="G41" s="21">
+        <f t="shared" si="13"/>
+        <v>1.3126233520170523</v>
+      </c>
+      <c r="L41">
+        <f>D41/D38</f>
+        <v>4.0553939002047636</v>
+      </c>
+      <c r="N41">
+        <f>F41/F38</f>
+        <v>1.3126233520170523</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <f>AVERAGE(L29:L41)</f>
+        <v>5.715003270729043</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
   </mergeCells>
-  <conditionalFormatting sqref="E23:E34 G23:G34">
+  <conditionalFormatting sqref="E26:E41 G26:G41">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -2835,7 +3407,653 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E23:E34 G23:G34</xm:sqref>
+          <xm:sqref>E26:E41 G26:G41</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE9CB73-5432-4CE0-9583-0D8A627C9947}">
+  <dimension ref="B1:L41"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="5" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1024</v>
+      </c>
+      <c r="D2">
+        <f>F2/1000</f>
+        <v>2.7594999999999998E-2</v>
+      </c>
+      <c r="F2">
+        <v>27.594999999999999</v>
+      </c>
+      <c r="H2">
+        <v>6.2013999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1024</v>
+      </c>
+      <c r="D3">
+        <f>F3/1000</f>
+        <v>1.0868000000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>10.868</v>
+      </c>
+      <c r="H3">
+        <v>8.1479999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1024</v>
+      </c>
+      <c r="D4">
+        <f>F4/1000</f>
+        <v>1.6095999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <v>16.096</v>
+      </c>
+      <c r="H4">
+        <v>6.6529999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>1024</v>
+      </c>
+      <c r="D5">
+        <f>F5/1000</f>
+        <v>1.3842000000000001E-3</v>
+      </c>
+      <c r="F5">
+        <v>1.3842000000000001</v>
+      </c>
+      <c r="H5">
+        <v>8.4968000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
+        <f>B2</f>
+        <v>std_vec_new</v>
+      </c>
+      <c r="C6">
+        <v>16384</v>
+      </c>
+      <c r="D6">
+        <f>F6/1000</f>
+        <v>1.6440999999999999</v>
+      </c>
+      <c r="F6">
+        <v>1644.1</v>
+      </c>
+      <c r="H6">
+        <v>155.61000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
+        <f t="shared" ref="B7:B17" si="0">B3</f>
+        <v>std_vec_with_exact_capacity</v>
+      </c>
+      <c r="C7">
+        <v>16384</v>
+      </c>
+      <c r="D7">
+        <f>F7/1000</f>
+        <v>0.75737999999999994</v>
+      </c>
+      <c r="F7">
+        <v>757.38</v>
+      </c>
+      <c r="H7">
+        <v>171.55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C8">
+        <v>16384</v>
+      </c>
+      <c r="D8">
+        <f>F8/1000</f>
+        <v>0.65244000000000002</v>
+      </c>
+      <c r="F8">
+        <v>652.44000000000005</v>
+      </c>
+      <c r="H8">
+        <v>157.63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C9">
+        <v>16384</v>
+      </c>
+      <c r="D9">
+        <f>F9/1000</f>
+        <v>2.1753999999999996E-3</v>
+      </c>
+      <c r="F9">
+        <v>2.1753999999999998</v>
+      </c>
+      <c r="H9">
+        <v>232.21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>std_vec_new</v>
+      </c>
+      <c r="C10">
+        <v>262144</v>
+      </c>
+      <c r="D10">
+        <v>26.672000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>std_vec_with_exact_capacity</v>
+      </c>
+      <c r="C11">
+        <v>262144</v>
+      </c>
+      <c r="D11">
+        <v>13.867000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C12">
+        <v>262144</v>
+      </c>
+      <c r="D12">
+        <v>13.747999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C13">
+        <v>262144</v>
+      </c>
+      <c r="D13">
+        <v>9.1730000000000006E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>std_vec_new</v>
+      </c>
+      <c r="C14">
+        <v>4194304</v>
+      </c>
+      <c r="D14">
+        <v>497.51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>std_vec_with_exact_capacity</v>
+      </c>
+      <c r="C15">
+        <v>4194304</v>
+      </c>
+      <c r="D15">
+        <v>224.62</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C16">
+        <v>4194304</v>
+      </c>
+      <c r="D16">
+        <v>227.58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C17">
+        <v>4194304</v>
+      </c>
+      <c r="D17">
+        <v>6.6280000000000002E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="38" t="str">
+        <f>C1</f>
+        <v>number of elements</v>
+      </c>
+      <c r="D25" s="39" t="str">
+        <f>D1</f>
+        <v>u64 x 1</v>
+      </c>
+      <c r="E25" s="40"/>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="41" t="str">
+        <f>B2</f>
+        <v>std_vec_new</v>
+      </c>
+      <c r="C26" s="9">
+        <f>C2</f>
+        <v>1024</v>
+      </c>
+      <c r="D26" s="10">
+        <f>D2</f>
+        <v>2.7594999999999998E-2</v>
+      </c>
+      <c r="E26" s="42">
+        <f>D26/D$26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="43" t="str">
+        <f t="shared" ref="B27:D41" si="1">B3</f>
+        <v>std_vec_with_exact_capacity</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="1"/>
+        <v>1024</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0868000000000001E-2</v>
+      </c>
+      <c r="E27" s="44">
+        <f t="shared" ref="E27:E29" si="2">D27/D$26</f>
+        <v>0.39383946367095496</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="1"/>
+        <v>1024</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6095999999999999E-2</v>
+      </c>
+      <c r="E28" s="44">
+        <f t="shared" si="2"/>
+        <v>0.58329407501358943</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C29" s="16">
+        <f t="shared" si="1"/>
+        <v>1024</v>
+      </c>
+      <c r="D29" s="17">
+        <f t="shared" si="1"/>
+        <v>1.3842000000000001E-3</v>
+      </c>
+      <c r="E29" s="46">
+        <f t="shared" si="2"/>
+        <v>5.016126109802501E-2</v>
+      </c>
+      <c r="J29">
+        <f>D29/D26</f>
+        <v>5.016126109802501E-2</v>
+      </c>
+      <c r="L29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="41" t="str">
+        <f t="shared" si="1"/>
+        <v>std_vec_new</v>
+      </c>
+      <c r="C30" s="9">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="D30" s="10">
+        <f t="shared" si="1"/>
+        <v>1.6440999999999999</v>
+      </c>
+      <c r="E30" s="42">
+        <f>D30/D$30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>std_vec_with_exact_capacity</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="1"/>
+        <v>0.75737999999999994</v>
+      </c>
+      <c r="E31" s="44">
+        <f t="shared" ref="E31:E33" si="3">D31/D$30</f>
+        <v>0.46066540964661518</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="1"/>
+        <v>0.65244000000000002</v>
+      </c>
+      <c r="E32" s="44">
+        <f t="shared" si="3"/>
+        <v>0.39683717535429724</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C33" s="16">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="D33" s="17">
+        <f t="shared" si="1"/>
+        <v>2.1753999999999996E-3</v>
+      </c>
+      <c r="E33" s="46">
+        <f t="shared" si="3"/>
+        <v>1.3231555258195972E-3</v>
+      </c>
+      <c r="J33">
+        <f>D33/D30</f>
+        <v>1.3231555258195972E-3</v>
+      </c>
+      <c r="L33" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="41" t="str">
+        <f t="shared" si="1"/>
+        <v>std_vec_new</v>
+      </c>
+      <c r="C34" s="9">
+        <f t="shared" si="1"/>
+        <v>262144</v>
+      </c>
+      <c r="D34" s="10">
+        <f t="shared" si="1"/>
+        <v>26.672000000000001</v>
+      </c>
+      <c r="E34" s="42">
+        <f>D34/D$34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>std_vec_with_exact_capacity</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="1"/>
+        <v>262144</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="1"/>
+        <v>13.867000000000001</v>
+      </c>
+      <c r="E35" s="44">
+        <f t="shared" ref="E35:E37" si="4">D35/D$34</f>
+        <v>0.51990851829634077</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="1"/>
+        <v>262144</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="1"/>
+        <v>13.747999999999999</v>
+      </c>
+      <c r="E36" s="44">
+        <f t="shared" si="4"/>
+        <v>0.5154469106178764</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C37" s="16">
+        <f t="shared" si="1"/>
+        <v>262144</v>
+      </c>
+      <c r="D37" s="17">
+        <f t="shared" si="1"/>
+        <v>9.1730000000000006E-3</v>
+      </c>
+      <c r="E37" s="46">
+        <f t="shared" si="4"/>
+        <v>3.4391871625674865E-4</v>
+      </c>
+      <c r="J37">
+        <f>D37/D34</f>
+        <v>3.4391871625674865E-4</v>
+      </c>
+      <c r="L37" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="41" t="str">
+        <f t="shared" si="1"/>
+        <v>std_vec_new</v>
+      </c>
+      <c r="C38" s="9">
+        <f t="shared" si="1"/>
+        <v>4194304</v>
+      </c>
+      <c r="D38" s="10">
+        <f t="shared" si="1"/>
+        <v>497.51</v>
+      </c>
+      <c r="E38" s="42">
+        <f>D38/D$38</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>std_vec_with_exact_capacity</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="1"/>
+        <v>4194304</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="1"/>
+        <v>224.62</v>
+      </c>
+      <c r="E39" s="44">
+        <f t="shared" ref="E39:E41" si="5">D39/D$38</f>
+        <v>0.45148841229322023</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>split_vec_doubling</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="1"/>
+        <v>4194304</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="1"/>
+        <v>227.58</v>
+      </c>
+      <c r="E40" s="44">
+        <f t="shared" si="5"/>
+        <v>0.4574380414464031</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="47" t="str">
+        <f t="shared" si="1"/>
+        <v>split_vec_recursive</v>
+      </c>
+      <c r="C41" s="48">
+        <f t="shared" si="1"/>
+        <v>4194304</v>
+      </c>
+      <c r="D41" s="49">
+        <f t="shared" si="1"/>
+        <v>6.6280000000000002E-3</v>
+      </c>
+      <c r="E41" s="50">
+        <f t="shared" si="5"/>
+        <v>1.3322345279491869E-5</v>
+      </c>
+      <c r="J41">
+        <f>D41/D38</f>
+        <v>1.3322345279491869E-5</v>
+      </c>
+      <c r="L41" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D25:E25"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E26:E41">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFCC3300"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EB8BD6CE-FEC1-4CA8-8DC9-599965DD1522}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EB8BD6CE-FEC1-4CA8-8DC9-599965DD1522}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E26:E41</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>